<commit_message>
Fixed test case, javadoc
</commit_message>
<xml_diff>
--- a/testdata/GroupedValues.xlsx
+++ b/testdata/GroupedValues.xlsx
@@ -10,7 +10,6 @@
     <sheet name="Test Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -383,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -399,7 +398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -439,8 +438,6 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>